<commit_message>
Move Some Excel Files
</commit_message>
<xml_diff>
--- a/database/Students.xlsx
+++ b/database/Students.xlsx
@@ -87,12 +87,25 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -167,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -179,6 +192,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,142 +537,142 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" s="10">
+      <c r="A3" s="12">
         <v>111111111</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="12">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A4" s="10">
+      <c r="A4" s="12">
         <v>222222222</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A5" s="10">
+      <c r="A5" s="12">
         <v>333333333</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="10">
+      <c r="A6" s="12">
         <v>444444444</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A7" s="10">
+      <c r="A7" s="12">
         <v>555555555</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" s="10">
+      <c r="A8" s="12">
         <v>666666666</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A9" s="10">
+      <c r="A9" s="12">
         <v>777777777</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" s="10">
+      <c r="A10" s="12">
         <v>888888888</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="10">
+      <c r="A11" s="12">
         <v>999999999</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>9</v>
       </c>
     </row>

</xml_diff>